<commit_message>
added erin's set for SPP
</commit_message>
<xml_diff>
--- a/Analysis.Tables.xlsx
+++ b/Analysis.Tables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KDValentine/Documents/GitHub/SPP-Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/SPP-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="126" documentId="11_34EB6FF0E67D412A609437AB59DE1BD5DCBE37E8" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{66FD1DCA-A522-7F43-B376-CDBA6D27BB8A}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="460" windowWidth="23780" windowHeight="14400" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOA200, other, ldt" sheetId="2" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="SOA1200, other, naming" sheetId="8" r:id="rId7"/>
     <sheet name="SOA1200, first, naming" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="82">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -203,11 +204,89 @@
   <si>
     <t>swow.p.fan_ss</t>
   </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>model.3a.a</t>
+  </si>
+  <si>
+    <t>model.3a.b</t>
+  </si>
+  <si>
+    <t>model.3b.a</t>
+  </si>
+  <si>
+    <t>model.3b.b</t>
+  </si>
+  <si>
+    <t>model3c.a</t>
+  </si>
+  <si>
+    <t>model3c.b</t>
+  </si>
+  <si>
+    <t>model3c.c</t>
+  </si>
+  <si>
+    <t>model3.2b.a</t>
+  </si>
+  <si>
+    <t>model3.2a.b</t>
+  </si>
+  <si>
+    <t>model3.2a.a</t>
+  </si>
+  <si>
+    <t>model3.2a.c</t>
+  </si>
+  <si>
+    <t>model3.2b.c</t>
+  </si>
+  <si>
+    <t>model3.2b.b</t>
+  </si>
+  <si>
+    <t>model3.2c.a</t>
+  </si>
+  <si>
+    <t>model3.2c.b</t>
+  </si>
+  <si>
+    <t>model3.2c.c</t>
+  </si>
+  <si>
+    <t>model4a.a</t>
+  </si>
+  <si>
+    <t>model4a.b</t>
+  </si>
+  <si>
+    <t>model4a.c</t>
+  </si>
+  <si>
+    <t>model4b.a</t>
+  </si>
+  <si>
+    <t>model4b.b</t>
+  </si>
+  <si>
+    <t>model4b.c</t>
+  </si>
+  <si>
+    <t>model4c.a</t>
+  </si>
+  <si>
+    <t>model4c.b</t>
+  </si>
+  <si>
+    <t>model4c.c</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -240,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +329,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,7 +353,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,6 +362,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -290,6 +381,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -557,10 +651,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1938,7 +2032,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
@@ -2892,7 +2986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3846,7 +3940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4800,7 +4894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
@@ -5754,7 +5848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6708,7 +6802,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7662,108 +7756,124 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AD26"/>
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="1">
+        <v>1.5610000000000001E-2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="P2" s="2" t="s">
         <v>13</v>
       </c>
@@ -7811,804 +7921,667 @@
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="B3" s="1">
+        <v>1.8360000000000001E-2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="B4" s="1">
+        <v>1.9359999999999999E-2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B5" s="1">
+        <v>1.941E-2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+    </row>
+    <row r="6" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    </row>
+    <row r="7" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B7" s="4">
+        <v>2.8340000000000001E-2</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="V8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W10" s="1"/>
-      <c r="X10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="Q11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD11" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3.1579999999999997E-2</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2.8420000000000001E-2</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="P11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD11" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" s="1"/>
-      <c r="X12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD12" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD13" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W14" s="1"/>
-      <c r="X14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD17" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD18" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD19" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD20" s="2" t="s">
-        <v>13</v>
+      <c r="B14" s="4">
+        <v>3.1710000000000002E-2</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="X14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD14" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD15" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="V17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD17" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>48</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-      <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
-      <c r="AD24" s="1"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>49</v>
-      </c>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
-      <c r="AA26" s="1"/>
-      <c r="AB26" s="1"/>
-      <c r="AC26" s="1"/>
-      <c r="AD26" s="1"/>
+      <c r="A21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.7289999999999997E-2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P21" s="2"/>
+      <c r="S21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W21" s="2"/>
+      <c r="Y21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+    </row>
+    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="1">
+        <v>4.2639999999999997E-2</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="S30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W30" s="2"/>
+      <c r="Y30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD30" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished regression and added to spreadsheet
</commit_message>
<xml_diff>
--- a/Analysis.Tables.xlsx
+++ b/Analysis.Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber Gillenwaters\Documents\GitHub\SPP-Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac924\Documents\GitHub\SPP-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BD3511-B80E-433E-BC10-EAA34252B887}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC83DB00-013A-4E01-B96D-68E9ECFF2F7F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="585" yWindow="465" windowWidth="23820" windowHeight="16005" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="585" yWindow="465" windowWidth="23820" windowHeight="16005" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOA200, other, ldt" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="67">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -271,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +290,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -305,7 +311,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,6 +332,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -612,14 +624,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.625" style="4" bestFit="1" customWidth="1"/>
@@ -1560,14 +1572,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.625" style="4" bestFit="1" customWidth="1"/>
@@ -1692,6 +1704,18 @@
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="4">
+        <v>6.7049999999999998E-2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1742,6 +1766,18 @@
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="B3" s="4">
+        <v>6.9849999999999995E-2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P3" s="6"/>
       <c r="Q3" s="4" t="s">
         <v>13</v>
@@ -1790,6 +1826,18 @@
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="B4" s="4">
+        <v>7.0180000000000006E-2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1837,6 +1885,24 @@
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="B5" s="4">
+        <v>7.2559999999999999E-2</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="R5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1881,10 +1947,28 @@
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B6" s="4">
+        <v>8.2540000000000002E-2</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="R6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="V6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1913,70 +1997,70 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="P7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD8" s="4" t="s">
+      <c r="V8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="W8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD8" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1984,9 +2068,30 @@
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="B9" s="4">
+        <v>8.5540000000000005E-2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="W9" s="4" t="s">
         <v>13</v>
@@ -2017,8 +2122,26 @@
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="B10" s="4">
+        <v>8.2680000000000003E-2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="Q10" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="V10" s="4" t="s">
         <v>13</v>
@@ -2049,9 +2172,30 @@
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B11" s="4">
+        <v>8.5589999999999999E-2</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="Q11" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="R11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="X11" s="4" t="s">
         <v>13</v>
       </c>
@@ -2074,181 +2218,181 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="P12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD12" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="P12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD12" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="P13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD13" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="P13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="P14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD14" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="P15" s="6"/>
-      <c r="W15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD15" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="P15" s="9"/>
+      <c r="W15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD15" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="V16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD16" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="V16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="X17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD17" s="4" t="s">
+      <c r="X17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD17" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2256,10 +2400,31 @@
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="B18" s="4">
+        <v>8.6050000000000001E-2</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="R18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="W18" s="4" t="s">
         <v>13</v>
       </c>
@@ -2273,146 +2438,146 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="Q19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD19" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="Q19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD19" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Q20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD20" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="Q20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD20" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="P21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD21" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="P21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD21" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="P22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD22" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="P22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD22" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="P23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD23" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="P23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD23" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="P24" s="6"/>
-      <c r="W24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="P24" s="9"/>
+      <c r="W24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD24" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="V25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD25" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="V25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD25" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AB26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD26" s="4" t="s">
+      <c r="AB26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD26" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2420,87 +2585,109 @@
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="B27" s="4">
+        <v>9.7439999999999999E-2</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="R27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T27" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="W27" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="AB27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD27" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="Q28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V28" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="Q28" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V28" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="Q29" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="Q29" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="P30" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W30" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="P30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="W30" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="P31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V31" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="P31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V31" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="P32" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="P32" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="P33" s="6"/>
-      <c r="W33" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="P33" s="9"/>
+      <c r="W33" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="V34" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="V34" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
KD analyses updated table
</commit_message>
<xml_diff>
--- a/Analysis.Tables.xlsx
+++ b/Analysis.Tables.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KDValentine/Documents/GitHub/SPP-Analysis/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="11440" yWindow="460" windowWidth="21740" windowHeight="14420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="SOA200, other, ldt" sheetId="2" r:id="rId1"/>
@@ -18,6 +23,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2396" uniqueCount="67">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -608,7 +616,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -618,11 +626,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD27" sqref="AD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" style="4" customWidth="1"/>
@@ -657,7 +665,7 @@
     <col min="31" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -746,10 +754,25 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="P2" s="4" t="s">
         <v>13</v>
       </c>
@@ -796,11 +819,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="6"/>
+      <c r="B3" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="Q3" s="4" t="s">
         <v>13</v>
       </c>
@@ -844,13 +884,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="B4" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P4" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="Q4" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="R4" s="4" t="s">
         <v>13</v>
       </c>
@@ -891,10 +949,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="B5" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="R5" s="4" t="s">
         <v>13</v>
       </c>
@@ -935,14 +1008,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="6"/>
+      <c r="B6" s="4">
+        <v>3.95E-2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="Q6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="T6" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="V6" s="4" t="s">
         <v>13</v>
       </c>
@@ -971,81 +1061,102 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30">
-      <c r="A8" s="4" t="s">
+      <c r="P7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30">
+      <c r="V8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P9" s="6"/>
+      <c r="B9" s="4">
+        <f>0.04279</f>
+        <v>4.2790000000000002E-2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="Q9" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="T9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="W9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1071,13 +1182,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="B10" s="4">
+        <v>4.0509999999999997E-2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="Q10" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="T10" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="V10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1103,13 +1232,34 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B11" s="4">
+        <v>4.2819999999999997E-2</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="Q11" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="T11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="X11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1132,195 +1282,218 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD12" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30">
-      <c r="A13" s="4" t="s">
+      <c r="P12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD13" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30">
-      <c r="A14" s="4" t="s">
+      <c r="P13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30">
-      <c r="A15" s="4" t="s">
+      <c r="P14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P15" s="6"/>
-      <c r="W15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD15" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30">
-      <c r="A16" s="4" t="s">
+      <c r="P15" s="7"/>
+      <c r="W15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="V16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD16" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30">
-      <c r="A17" s="4" t="s">
+      <c r="V16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="X17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD17" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30">
+      <c r="X17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="P18" s="6"/>
+      <c r="B18" s="4">
+        <v>5.101E-2</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="Q18" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="V18" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="W18" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="Y18" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="AB18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1331,153 +1504,168 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Q19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD19" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30">
-      <c r="A20" s="4" t="s">
+      <c r="Q19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Q20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD20" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30">
-      <c r="A21" s="4" t="s">
+      <c r="Q20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="P21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD21" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30">
-      <c r="A22" s="4" t="s">
+      <c r="P21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="P22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD22" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30">
-      <c r="A23" s="4" t="s">
+      <c r="P22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="P23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD23" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30">
-      <c r="A24" s="4" t="s">
+      <c r="P23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="P24" s="6"/>
-      <c r="W24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30">
-      <c r="A25" s="4" t="s">
+      <c r="P24" s="7"/>
+      <c r="W24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="V25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD25" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30">
-      <c r="A26" s="4" t="s">
+      <c r="V25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD25" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AB26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD26" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30">
+      <c r="AB26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="B27" s="4">
+        <v>6.2960000000000002E-2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="4" t="s">
         <v>13</v>
@@ -1485,85 +1673,89 @@
       <c r="W27" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:30">
-      <c r="A28" s="4" t="s">
+      <c r="Y27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD27" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Q28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V28" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30">
-      <c r="A29" s="4" t="s">
+      <c r="Q28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q29" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30">
-      <c r="A30" s="4" t="s">
+      <c r="Q29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="P30" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W30" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30">
-      <c r="A31" s="4" t="s">
+      <c r="P30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="P31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V31" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30">
-      <c r="A32" s="4" t="s">
+      <c r="P31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V31" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="P32" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23">
-      <c r="A33" s="4" t="s">
+      <c r="P32" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="P33" s="6"/>
-      <c r="W33" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23">
-      <c r="A34" s="4" t="s">
+      <c r="P33" s="7"/>
+      <c r="W33" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="V34" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23">
-      <c r="A35" s="4" t="s">
+      <c r="V34" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1571,11 +1763,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="4" customWidth="1"/>
@@ -1610,7 +1802,7 @@
     <col min="31" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -1699,7 +1891,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1761,7 +1953,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1821,7 +2013,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -1880,7 +2072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1942,7 +2134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1996,7 +2188,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="8" customFormat="1">
+    <row r="7" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
@@ -2031,7 +2223,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="8" customFormat="1">
+    <row r="8" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
@@ -2063,7 +2255,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -2117,7 +2309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -2167,7 +2359,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -2217,7 +2409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="8" customFormat="1">
+    <row r="12" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>43</v>
       </c>
@@ -2249,7 +2441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="8" customFormat="1">
+    <row r="13" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>44</v>
       </c>
@@ -2281,7 +2473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="8" customFormat="1">
+    <row r="14" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
@@ -2310,7 +2502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="8" customFormat="1">
+    <row r="15" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>45</v>
       </c>
@@ -2340,7 +2532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="8" customFormat="1">
+    <row r="16" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>46</v>
       </c>
@@ -2369,7 +2561,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="8" customFormat="1">
+    <row r="17" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>47</v>
       </c>
@@ -2395,7 +2587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -2437,7 +2629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="8" customFormat="1">
+    <row r="19" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>49</v>
       </c>
@@ -2457,7 +2649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="8" customFormat="1">
+    <row r="20" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>51</v>
       </c>
@@ -2474,7 +2666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="8" customFormat="1">
+    <row r="21" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>48</v>
       </c>
@@ -2494,7 +2686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="8" customFormat="1">
+    <row r="22" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>53</v>
       </c>
@@ -2514,7 +2706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="8" customFormat="1">
+    <row r="23" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>52</v>
       </c>
@@ -2531,7 +2723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="8" customFormat="1">
+    <row r="24" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>54</v>
       </c>
@@ -2549,7 +2741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="8" customFormat="1">
+    <row r="25" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>55</v>
       </c>
@@ -2566,7 +2758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="8" customFormat="1">
+    <row r="26" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>56</v>
       </c>
@@ -2580,7 +2772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -2613,7 +2805,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="8" customFormat="1">
+    <row r="28" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>58</v>
       </c>
@@ -2624,7 +2816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="8" customFormat="1">
+    <row r="29" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>59</v>
       </c>
@@ -2632,7 +2824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="8" customFormat="1">
+    <row r="30" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>60</v>
       </c>
@@ -2643,7 +2835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="8" customFormat="1">
+    <row r="31" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>61</v>
       </c>
@@ -2654,7 +2846,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="8" customFormat="1">
+    <row r="32" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>62</v>
       </c>
@@ -2662,7 +2854,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="8" customFormat="1">
+    <row r="33" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>63</v>
       </c>
@@ -2671,7 +2863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="8" customFormat="1">
+    <row r="34" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>64</v>
       </c>
@@ -2679,7 +2871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="8" customFormat="1">
+    <row r="35" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>65</v>
       </c>
@@ -2687,11 +2879,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2703,7 +2890,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
@@ -2738,7 +2925,7 @@
     <col min="31" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -2827,7 +3014,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -2877,7 +3064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -2925,7 +3112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -2972,7 +3159,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -3016,7 +3203,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -3052,7 +3239,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -3087,7 +3274,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -3119,7 +3306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -3152,7 +3339,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -3184,7 +3371,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -3213,7 +3400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -3245,7 +3432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>44</v>
       </c>
@@ -3277,7 +3464,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -3306,7 +3493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
@@ -3336,7 +3523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
@@ -3365,7 +3552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>47</v>
       </c>
@@ -3391,7 +3578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -3412,7 +3599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -3432,7 +3619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>51</v>
       </c>
@@ -3449,7 +3636,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -3469,7 +3656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>53</v>
       </c>
@@ -3489,7 +3676,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>52</v>
       </c>
@@ -3506,7 +3693,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
@@ -3524,7 +3711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>55</v>
       </c>
@@ -3541,7 +3728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>56</v>
       </c>
@@ -3555,7 +3742,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -3567,7 +3754,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>58</v>
       </c>
@@ -3578,7 +3765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>59</v>
       </c>
@@ -3586,7 +3773,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>60</v>
       </c>
@@ -3597,7 +3784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
@@ -3608,7 +3795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>62</v>
       </c>
@@ -3616,7 +3803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>63</v>
       </c>
@@ -3625,7 +3812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>64</v>
       </c>
@@ -3633,18 +3820,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3652,11 +3834,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -3691,7 +3873,7 @@
     <col min="31" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -3780,7 +3962,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -3848,7 +4030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -3914,7 +4096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -3979,7 +4161,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -4038,7 +4220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -4098,7 +4280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="2" customFormat="1">
+    <row r="7" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4133,7 +4315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="2" customFormat="1">
+    <row r="8" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -4165,7 +4347,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -4225,7 +4407,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -4281,7 +4463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -4337,7 +4519,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="2" customFormat="1">
+    <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -4369,7 +4551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="2" customFormat="1">
+    <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -4401,7 +4583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="2" customFormat="1">
+    <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -4430,7 +4612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="2" customFormat="1">
+    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -4460,7 +4642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="2" customFormat="1">
+    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -4489,7 +4671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="2" customFormat="1">
+    <row r="17" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -4515,7 +4697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -4563,7 +4745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="2" customFormat="1">
+    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -4583,7 +4765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="2" customFormat="1">
+    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -4600,7 +4782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="2" customFormat="1">
+    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
@@ -4620,7 +4802,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="2" customFormat="1">
+    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
@@ -4640,7 +4822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="2" customFormat="1">
+    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
@@ -4657,7 +4839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="2" customFormat="1">
+    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -4675,7 +4857,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="2" customFormat="1">
+    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -4692,7 +4874,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="2" customFormat="1">
+    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -4706,7 +4888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -4751,7 +4933,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="2" customFormat="1">
+    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
@@ -4762,7 +4944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="2" customFormat="1">
+    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
@@ -4770,7 +4952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="2" customFormat="1">
+    <row r="30" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
@@ -4781,7 +4963,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="2" customFormat="1">
+    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
@@ -4792,7 +4974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="2" customFormat="1">
+    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -4800,7 +4982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="2" customFormat="1">
+    <row r="33" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
@@ -4809,7 +4991,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="2" customFormat="1">
+    <row r="34" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -4817,18 +4999,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="2" customFormat="1">
+    <row r="35" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4840,7 +5017,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
@@ -4875,7 +5052,7 @@
     <col min="31" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -4964,7 +5141,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -5014,7 +5191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -5062,7 +5239,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -5109,7 +5286,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -5153,7 +5330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -5189,7 +5366,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -5224,7 +5401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -5256,7 +5433,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -5289,7 +5466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -5321,7 +5498,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -5350,7 +5527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -5382,7 +5559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>44</v>
       </c>
@@ -5414,7 +5591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -5443,7 +5620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
@@ -5473,7 +5650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
@@ -5502,7 +5679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>47</v>
       </c>
@@ -5528,7 +5705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -5549,7 +5726,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -5569,7 +5746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>51</v>
       </c>
@@ -5586,7 +5763,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -5606,7 +5783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>53</v>
       </c>
@@ -5626,7 +5803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>52</v>
       </c>
@@ -5643,7 +5820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
@@ -5661,7 +5838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>55</v>
       </c>
@@ -5678,7 +5855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>56</v>
       </c>
@@ -5692,7 +5869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -5704,7 +5881,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>58</v>
       </c>
@@ -5715,7 +5892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>59</v>
       </c>
@@ -5723,7 +5900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>60</v>
       </c>
@@ -5734,7 +5911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
@@ -5745,7 +5922,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>62</v>
       </c>
@@ -5753,7 +5930,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>63</v>
       </c>
@@ -5762,7 +5939,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>64</v>
       </c>
@@ -5770,18 +5947,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5793,7 +5965,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -5828,7 +6000,7 @@
     <col min="31" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -5917,7 +6089,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -5979,7 +6151,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -6044,7 +6216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -6106,7 +6278,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -6162,7 +6334,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -6216,7 +6388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -6270,7 +6442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -6322,7 +6494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -6374,7 +6546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -6426,7 +6598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -6476,7 +6648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>66</v>
       </c>
@@ -6499,7 +6671,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
@@ -6551,7 +6723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -6603,7 +6775,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
@@ -6653,7 +6825,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -6703,7 +6875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -6753,7 +6925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -6801,7 +6973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>50</v>
       </c>
@@ -6845,7 +7017,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
@@ -6889,7 +7061,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>51</v>
       </c>
@@ -6927,7 +7099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>48</v>
       </c>
@@ -6971,7 +7143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>53</v>
       </c>
@@ -7015,7 +7187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
@@ -7057,7 +7229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>54</v>
       </c>
@@ -7099,7 +7271,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>55</v>
       </c>
@@ -7141,7 +7313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>56</v>
       </c>
@@ -7181,7 +7353,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
@@ -7219,7 +7391,7 @@
       <c r="AC28" s="2"/>
       <c r="AD28" s="2"/>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>58</v>
       </c>
@@ -7257,7 +7429,7 @@
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>59</v>
       </c>
@@ -7286,7 +7458,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>60</v>
       </c>
@@ -7324,7 +7496,7 @@
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>61</v>
       </c>
@@ -7362,7 +7534,7 @@
       <c r="AC32" s="2"/>
       <c r="AD32" s="2"/>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>62</v>
       </c>
@@ -7398,7 +7570,7 @@
       <c r="AC33" s="2"/>
       <c r="AD33" s="2"/>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>63</v>
       </c>
@@ -7434,7 +7606,7 @@
       <c r="AC34" s="2"/>
       <c r="AD34" s="2"/>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>64</v>
       </c>
@@ -7470,7 +7642,7 @@
       <c r="AC35" s="2"/>
       <c r="AD35" s="2"/>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>65</v>
       </c>
@@ -7506,11 +7678,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7523,7 +7690,7 @@
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="4" customWidth="1"/>
@@ -7558,7 +7725,7 @@
     <col min="31" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -7647,7 +7814,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -7706,7 +7873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -7766,7 +7933,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -7825,7 +7992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -7881,7 +8048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -7935,7 +8102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -7970,7 +8137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -8002,7 +8169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -8053,7 +8220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -8103,7 +8270,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -8150,7 +8317,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -8182,7 +8349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>44</v>
       </c>
@@ -8214,7 +8381,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -8243,7 +8410,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
@@ -8273,7 +8440,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
@@ -8302,7 +8469,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>47</v>
       </c>
@@ -8328,7 +8495,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -8367,7 +8534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -8393,7 +8560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>51</v>
       </c>
@@ -8410,7 +8577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -8430,7 +8597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>53</v>
       </c>
@@ -8450,7 +8617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>52</v>
       </c>
@@ -8467,7 +8634,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
@@ -8485,7 +8652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>55</v>
       </c>
@@ -8502,7 +8669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>56</v>
       </c>
@@ -8516,7 +8683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -8546,7 +8713,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>58</v>
       </c>
@@ -8557,7 +8724,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>59</v>
       </c>
@@ -8565,7 +8732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>60</v>
       </c>
@@ -8576,7 +8743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
@@ -8587,7 +8754,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>62</v>
       </c>
@@ -8595,7 +8762,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>63</v>
       </c>
@@ -8604,7 +8771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>64</v>
       </c>
@@ -8612,18 +8779,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8635,13 +8797,13 @@
       <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -8730,7 +8892,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -8792,7 +8954,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -8826,7 +8988,7 @@
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -8863,7 +9025,7 @@
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -8893,12 +9055,12 @@
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
     </row>
-    <row r="6" spans="1:30" s="5" customFormat="1">
+    <row r="6" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="4" customFormat="1">
+    <row r="7" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -8951,7 +9113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="5" customFormat="1">
+    <row r="8" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -8983,7 +9145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="5" customFormat="1">
+    <row r="9" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
@@ -9015,7 +9177,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="5" customFormat="1">
+    <row r="10" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
@@ -9047,7 +9209,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="5" customFormat="1">
+    <row r="11" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -9076,7 +9238,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="4" customFormat="1">
+    <row r="12" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -9126,7 +9288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="4" customFormat="1">
+    <row r="13" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>44</v>
       </c>
@@ -9176,7 +9338,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="4" customFormat="1">
+    <row r="14" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -9223,7 +9385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="5" customFormat="1">
+    <row r="15" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>45</v>
       </c>
@@ -9252,7 +9414,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="5" customFormat="1">
+    <row r="16" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
@@ -9281,7 +9443,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="5" customFormat="1">
+    <row r="17" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>47</v>
       </c>
@@ -9310,22 +9472,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" s="2" customFormat="1">
+    <row r="18" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="2" customFormat="1">
+    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="2" customFormat="1">
+    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -9359,47 +9521,47 @@
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
     </row>
-    <row r="22" spans="1:30" s="2" customFormat="1">
+    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="2" customFormat="1">
+    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="2" customFormat="1">
+    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="2" customFormat="1">
+    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="2" customFormat="1">
+    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:30" s="2" customFormat="1">
+    <row r="27" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="2" customFormat="1">
+    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="2" customFormat="1">
+    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>60</v>
       </c>
@@ -9430,37 +9592,32 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="2" customFormat="1">
+    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="2" customFormat="1">
+    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:1" s="2" customFormat="1">
+    <row r="33" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:1" s="2" customFormat="1">
+    <row r="34" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:1" s="2" customFormat="1">
+    <row r="35" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Table updated for 1200/other/ldt
</commit_message>
<xml_diff>
--- a/Analysis.Tables.xlsx
+++ b/Analysis.Tables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KDValentine/Documents/GitHub/SPP-Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/addiew/Documents/SPP-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742FA932-CA9F-2E4D-9241-C77629467003}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11440" yWindow="460" windowWidth="21740" windowHeight="14420" tabRatio="500"/>
+    <workbookView xWindow="13180" yWindow="460" windowWidth="21740" windowHeight="14420" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOA200, other, ldt" sheetId="2" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="SOA1200, other, naming" sheetId="8" r:id="rId7"/>
     <sheet name="SOA1200, first, naming" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2396" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2446" uniqueCount="67">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -240,7 +241,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -623,10 +624,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="AD27" sqref="AD27"/>
     </sheetView>
   </sheetViews>
@@ -1760,7 +1761,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2883,7 +2884,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3831,10 +3832,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -5010,11 +5011,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5145,6 +5146,18 @@
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P2" s="4" t="s">
         <v>13</v>
       </c>
@@ -5195,7 +5208,24 @@
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="6"/>
+      <c r="B3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="Q3" s="4" t="s">
         <v>13</v>
       </c>
@@ -5243,8 +5273,23 @@
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="B4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P4" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>13</v>
@@ -5290,6 +5335,18 @@
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="R5" s="4" t="s">
         <v>13</v>
       </c>
@@ -5334,7 +5391,24 @@
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="6"/>
+      <c r="B6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="Q6" s="4" t="s">
         <v>13</v>
       </c>
@@ -5366,70 +5440,70 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="P7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD8" s="4" t="s">
+      <c r="V8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5437,9 +5511,29 @@
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P9" s="6"/>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="Q9" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="W9" s="4" t="s">
         <v>13</v>
@@ -5470,6 +5564,24 @@
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="B10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="Q10" s="4" t="s">
         <v>13</v>
       </c>
@@ -5502,6 +5614,24 @@
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="Q11" s="4" t="s">
         <v>13</v>
       </c>
@@ -5527,345 +5657,345 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD12" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="P12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD13" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="P13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="P14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P15" s="6"/>
-      <c r="W15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD15" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="P15" s="7"/>
+      <c r="W15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="V16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD16" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="V16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="X17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD17" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="X17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD18" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="P18" s="7"/>
+      <c r="Q18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Q19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD19" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="Q19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Q20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD20" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="Q20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="P21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD21" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="P21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="P22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD22" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="P22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="P23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD23" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="P23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="P24" s="6"/>
-      <c r="W24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="P24" s="7"/>
+      <c r="W24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="V25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD25" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="V25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD25" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AB26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD26" s="4" t="s">
+      <c r="AB26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD26" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5873,7 +6003,24 @@
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="P27" s="6"/>
+      <c r="B27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="Q27" s="4" t="s">
         <v>13</v>
       </c>
@@ -5881,74 +6028,74 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Q28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V28" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="Q28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q29" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="Q29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="P30" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W30" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="P30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="P31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V31" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="P31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V31" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="P32" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="P32" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="P33" s="6"/>
-      <c r="W33" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="P33" s="7"/>
+      <c r="W33" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="V34" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="V34" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5958,7 +6105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD36"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -7682,7 +7829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8790,7 +8937,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>